<commit_message>
committing to be able to git pull
</commit_message>
<xml_diff>
--- a/Doc/scRnaSeqScheduleDev.xlsx
+++ b/Doc/scRnaSeqScheduleDev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baller01/MyProjectsSvn/SvnRepoForTraining/BioinfoCore/FernandesM/20200511_FernandesM_ME_crukBiSs2020/trunk/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210ABAE5-54BF-9A4B-9FD5-B9C10CFA6823}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969B956F-A379-F64B-B1CD-537C9BDBA3A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="460" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="500" windowWidth="18640" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Daily Schedule</t>
   </si>
@@ -89,25 +89,22 @@
     <t>dimRedForViz + confounding factors (?) - Zeynep</t>
   </si>
   <si>
-    <t>batch correction (GSM3872434) - Abbi</t>
-  </si>
-  <si>
     <t>batch correction (GSM3872434) + data set integration - Abbi</t>
   </si>
   <si>
+    <t>intro - Kasia + Preamble - Stephane</t>
+  </si>
+  <si>
+    <t>seq QC + cellranger - Ash</t>
+  </si>
+  <si>
     <t>data set integration- Abbi</t>
   </si>
   <si>
-    <t>clustering - Zeynep</t>
-  </si>
-  <si>
-    <t>cluster marker genes - Stephane</t>
-  </si>
-  <si>
-    <t>intro - Kasia + Preamble - Stephane</t>
-  </si>
-  <si>
-    <t>seq QC + cellranger - Ash</t>
+    <t>clustering - Stephane</t>
+  </si>
+  <si>
+    <t>cluster marker genes - Zeynep</t>
   </si>
 </sst>
 </file>
@@ -613,8 +610,8 @@
   </sheetPr>
   <dimension ref="B1:J52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -861,7 +858,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -877,7 +874,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -893,7 +890,7 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -909,7 +906,7 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -963,7 +960,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -976,12 +973,12 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -994,12 +991,12 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -1012,12 +1009,12 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">

</xml_diff>